<commit_message>
link to csv version of patient data
</commit_message>
<xml_diff>
--- a/patient-data.xlsx
+++ b/patient-data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UOS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\data-formatting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="7035"/>
   </bookViews>
   <sheets>
     <sheet name="patient-data" sheetId="1" r:id="rId1"/>
@@ -2241,11 +2241,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2267,7 +2273,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -2289,7 +2295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>42339</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2374,7 +2380,7 @@
         <v>-1.31</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2415,7 +2421,7 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2497,7 +2503,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2579,7 +2585,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -2620,7 +2626,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>-1.43</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>42369</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>-2.41</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -2828,7 +2834,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>-0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -2910,7 +2916,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -2951,7 +2957,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -2992,7 +2998,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>-1.97</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -3074,7 +3080,7 @@
         <v>-1.18</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -3115,7 +3121,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -3197,7 +3203,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -3282,7 +3288,7 @@
         <v>42400</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>144</v>
       </c>
@@ -3323,7 +3329,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -3364,7 +3370,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>153</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>158</v>
       </c>
@@ -3446,7 +3452,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>163</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>42431</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -3531,7 +3537,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>171</v>
       </c>
@@ -3572,7 +3578,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>176</v>
       </c>
@@ -3613,7 +3619,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>180</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>185</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -3736,7 +3742,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>194</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>42460</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>198</v>
       </c>
@@ -3821,7 +3827,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>202</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>-2.17</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>208</v>
       </c>
@@ -3903,7 +3909,7 @@
         <v>-1.32</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -3944,7 +3950,7 @@
         <v>-1.89</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>218</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>222</v>
       </c>
@@ -4026,7 +4032,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>226</v>
       </c>
@@ -4067,7 +4073,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>230</v>
       </c>
@@ -4108,7 +4114,7 @@
         <v>-1.21</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>234</v>
       </c>
@@ -4149,7 +4155,7 @@
         <v>-0.66</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -4193,7 +4199,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>243</v>
       </c>
@@ -4234,7 +4240,7 @@
         <v>-0.32</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>247</v>
       </c>
@@ -4275,7 +4281,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>252</v>
       </c>
@@ -4316,7 +4322,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>256</v>
       </c>
@@ -4357,7 +4363,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>260</v>
       </c>
@@ -4398,7 +4404,7 @@
         <v>-0.74</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>264</v>
       </c>
@@ -4439,7 +4445,7 @@
         <v>-1.07</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>269</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>273</v>
       </c>
@@ -4524,7 +4530,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>277</v>
       </c>
@@ -4565,7 +4571,7 @@
         <v>-1.21</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>281</v>
       </c>
@@ -4606,7 +4612,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>286</v>
       </c>
@@ -4647,7 +4653,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>292</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>296</v>
       </c>
@@ -4729,7 +4735,7 @@
         <v>-2.36</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>301</v>
       </c>
@@ -4773,7 +4779,7 @@
         <v>42552</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>306</v>
       </c>
@@ -4814,7 +4820,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>310</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>314</v>
       </c>
@@ -4896,7 +4902,7 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>318</v>
       </c>
@@ -4937,7 +4943,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>323</v>
       </c>
@@ -4981,7 +4987,7 @@
         <v>42582</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>326</v>
       </c>
@@ -5022,7 +5028,7 @@
         <v>-1.06</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>330</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>335</v>
       </c>
@@ -5104,7 +5110,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>339</v>
       </c>
@@ -5145,7 +5151,7 @@
         <v>-1.46</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>343</v>
       </c>
@@ -5186,7 +5192,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>348</v>
       </c>
@@ -5227,7 +5233,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>353</v>
       </c>
@@ -5268,7 +5274,7 @@
         <v>-3.14</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>357</v>
       </c>
@@ -5309,7 +5315,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>361</v>
       </c>
@@ -5350,7 +5356,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>366</v>
       </c>
@@ -5391,7 +5397,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>370</v>
       </c>
@@ -5432,7 +5438,7 @@
         <v>-0.81</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>374</v>
       </c>
@@ -5476,7 +5482,7 @@
         <v>42613</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>378</v>
       </c>
@@ -5517,7 +5523,7 @@
         <v>-1.41</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>382</v>
       </c>
@@ -5558,7 +5564,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>386</v>
       </c>
@@ -5599,7 +5605,7 @@
         <v>-0.99</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>390</v>
       </c>
@@ -5640,7 +5646,7 @@
         <v>-0.92</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>394</v>
       </c>
@@ -5681,7 +5687,7 @@
         <v>-0.28000000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>398</v>
       </c>
@@ -5722,7 +5728,7 @@
         <v>-1.18</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>402</v>
       </c>
@@ -5763,7 +5769,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>407</v>
       </c>
@@ -5804,7 +5810,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>411</v>
       </c>
@@ -5845,7 +5851,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>415</v>
       </c>
@@ -5889,7 +5895,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>419</v>
       </c>
@@ -5930,7 +5936,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>423</v>
       </c>
@@ -5971,7 +5977,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>428</v>
       </c>
@@ -6012,7 +6018,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>432</v>
       </c>
@@ -6053,7 +6059,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>436</v>
       </c>
@@ -6094,7 +6100,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>440</v>
       </c>
@@ -6135,7 +6141,7 @@
         <v>-1.07</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>444</v>
       </c>
@@ -6176,7 +6182,7 @@
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>447</v>
       </c>
@@ -6220,7 +6226,7 @@
         <v>42674</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>451</v>
       </c>
@@ -6261,7 +6267,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>455</v>
       </c>
@@ -6302,7 +6308,7 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>459</v>
       </c>
@@ -6343,7 +6349,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>463</v>
       </c>
@@ -6384,7 +6390,7 @@
         <v>-0.78</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>467</v>
       </c>
@@ -6427,5 +6433,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>